<commit_message>
Formato inspecciones y cambios menores
</commit_message>
<xml_diff>
--- a/public/importacion/Plantilla Matriz Riesgo.xlsx
+++ b/public/importacion/Plantilla Matriz Riesgo.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$8:$Y$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$8:$S$8</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Sisoft - Matriz de Riesgo</t>
   </si>
@@ -69,33 +69,15 @@
     <t>Temporal</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Fuente</t>
   </si>
   <si>
     <t>Nivel Exposicion</t>
   </si>
   <si>
-    <t>Nivel Probabilidad</t>
-  </si>
-  <si>
-    <t>Interpretacion Probabilida</t>
-  </si>
-  <si>
     <t>Nivel Consencuencia</t>
   </si>
   <si>
-    <t>Nivel Riesgo</t>
-  </si>
-  <si>
-    <t>Interpretacion Riesgo</t>
-  </si>
-  <si>
-    <t>Aceptacion Riesgo</t>
-  </si>
-  <si>
     <t>Eliminacion</t>
   </si>
   <si>
@@ -132,9 +114,6 @@
     <t>temporalesMatrizRiesgoDetalle</t>
   </si>
   <si>
-    <t>totalExpuestosMatrizRiesgoDetalle</t>
-  </si>
-  <si>
     <t>fuenteMatrizRiesgoDetalle</t>
   </si>
   <si>
@@ -165,30 +144,15 @@
     <t>nivelExposicionMatrizRiesgoDetalle</t>
   </si>
   <si>
-    <t>nivelProbabilidadMatrizRiesgoDetalle</t>
-  </si>
-  <si>
-    <t>nombreProbabilidadMatrizRiesgoDetalle</t>
-  </si>
-  <si>
     <t>sustitucionMatrizRiesgoDetalle</t>
   </si>
   <si>
     <t>eliminacionMatrizRiesgoDetalle</t>
   </si>
   <si>
-    <t>aceptacionRiesgoMatrizRiesgoDetalle</t>
-  </si>
-  <si>
-    <t>nombreRiesgoMatrizRiesgoDetalle</t>
-  </si>
-  <si>
     <t>nivelConsecuenciaMatrizRiesgoDetalle</t>
   </si>
   <si>
-    <t>nivelRiesgoMatrizRiesgoDetalle</t>
-  </si>
-  <si>
     <t>controlMatrizRiesgoDetalle</t>
   </si>
   <si>
@@ -210,9 +174,6 @@
     <t>EVALUACIÓN DE RIESGO</t>
   </si>
   <si>
-    <t>VALORACION</t>
-  </si>
-  <si>
     <t>MEDIDAS DE INTERVENCION</t>
   </si>
   <si>
@@ -220,13 +181,49 @@
   </si>
   <si>
     <t>Nivel Deficiencia</t>
+  </si>
+  <si>
+    <t>Volumen alto de aparatos telefónicos y de comunicación usados (celulares, audífonos, radios, etc.)</t>
+  </si>
+  <si>
+    <t>Disconfot, cefalea, falta de concentracion</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Eli</t>
+  </si>
+  <si>
+    <t>Sus</t>
+  </si>
+  <si>
+    <t>Con</t>
+  </si>
+  <si>
+    <t>Guantes</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>2016-09-20</t>
+  </si>
+  <si>
+    <t>prueba nueva andres</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +251,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -351,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -363,6 +366,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -375,10 +382,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,80 +684,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.75" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -764,65 +756,65 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U7" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="5"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="C7" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="7" t="s">
@@ -835,16 +827,16 @@
         <v>16</v>
       </c>
       <c r="J8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>18</v>
@@ -861,121 +853,139 @@
       <c r="R8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="S8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="T8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="U8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="V8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="W8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="X8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y8" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="I9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="J9" t="s">
         <v>34</v>
       </c>
-      <c r="G9" t="s">
+      <c r="K9" t="s">
         <v>35</v>
       </c>
-      <c r="H9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" t="s">
         <v>41</v>
       </c>
-      <c r="L9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="Q9" t="s">
+        <v>44</v>
+      </c>
+      <c r="R9" t="s">
+        <v>45</v>
+      </c>
+      <c r="S9" t="s">
         <v>46</v>
       </c>
-      <c r="N9" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q9" t="s">
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E10" t="s">
         <v>54</v>
       </c>
-      <c r="R9" t="s">
+      <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="S9" t="s">
-        <v>53</v>
-      </c>
-      <c r="T9" t="s">
-        <v>52</v>
-      </c>
-      <c r="U9" t="s">
-        <v>51</v>
-      </c>
-      <c r="V9" t="s">
-        <v>50</v>
-      </c>
-      <c r="W9" t="s">
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
         <v>56</v>
       </c>
-      <c r="X9" t="s">
+      <c r="J10" t="s">
         <v>57</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="K10" t="s">
         <v>58</v>
       </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>4</v>
+      </c>
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10" t="s">
+        <v>59</v>
+      </c>
+      <c r="P10" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>61</v>
+      </c>
+      <c r="R10" t="s">
+        <v>62</v>
+      </c>
+      <c r="S10" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A8:Y8"/>
+  <autoFilter ref="A8:S8"/>
   <dataConsolidate/>
   <mergeCells count="6">
-    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="A1:Q1"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:S7"/>
-    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O7:R7"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I10">
-      <formula1>G10+H10</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <extLst>
@@ -985,19 +995,19 @@
           <x14:formula1>
             <xm:f>lista!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>M10</xm:sqref>
+          <xm:sqref>L10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lista!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>N10</xm:sqref>
+          <xm:sqref>M10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lista!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>Q10</xm:sqref>
+          <xm:sqref>N10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -1021,23 +1031,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>